<commit_message>
1. Animaiton Effect 주석 처리
</commit_message>
<xml_diff>
--- a/스타듀밸리_Win32API_김다인.xlsx
+++ b/스타듀밸리_Win32API_김다인.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\StardewVelly_InnyEngine_Win32API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF85BA4-20C5-47AB-90CA-0A249A43F289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369EB57B-E252-4FD8-B5C0-F5DBB198BD0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{DAD171CC-0285-4BF8-BECE-3F60597F3648}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{DAD171CC-0285-4BF8-BECE-3F60597F3648}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="180">
   <si>
     <t>게임명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -251,10 +251,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Charator</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Sound</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -275,10 +271,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>마을주민</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Animals</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -287,22 +279,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>고양이</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>강아지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Monster</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Environment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>나무</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -315,65 +291,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>집</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>바다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>길</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Other</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Tilesets</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Loge</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Title Screen</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Mail</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Tools</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Weapons</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>Ambience</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Charactors</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Interface</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Miscellaneous</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>O</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -768,6 +693,90 @@
   </si>
   <si>
     <t>모이먹기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Scene 정리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resource 정리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플레이어 조작키 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASDW / 마우스 좌, 우측 키</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intro Scene 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Title Scene 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FSM 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장비 기준 / 방향 기준</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몬스터 FSM 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPC FSM 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플레이어 알람 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인벤토리 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시스템 시간 환경 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>돌 캐기, 채집하기, 농사짓기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플레이어 Action 구현 - 농사 및 채집</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플레이어 Action 구현 - 사냥</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몬스터 FSM 구현, 사냥 Action 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카메라 셋팅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상점 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플레이어 Action 구현 - 낚시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>in game 오전 6시 ~ 새벽 2시 (20시간) - 10분</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -969,7 +978,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1045,6 +1054,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1057,11 +1072,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1377,10 +1389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F83BC03-76F3-4346-9745-B89DC329662E}">
-  <dimension ref="B2:E53"/>
+  <dimension ref="B2:K74"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A60" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1393,7 +1405,7 @@
     <col min="6" max="6" width="4.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
@@ -1403,7 +1415,7 @@
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
     </row>
-    <row r="3" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="7" t="s">
         <v>3</v>
       </c>
@@ -1412,8 +1424,11 @@
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
-    </row>
-    <row r="4" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="H3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
@@ -1422,16 +1437,27 @@
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
-    </row>
-    <row r="5" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="H4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="7" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="H5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="H6" s="31" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B7" s="7" t="s">
         <v>4</v>
       </c>
@@ -1444,8 +1470,14 @@
       <c r="E7" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="H7" t="s">
+        <v>161</v>
+      </c>
+      <c r="K7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B8" s="6" t="s">
         <v>42</v>
       </c>
@@ -1456,8 +1488,14 @@
       <c r="E8" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="H8" t="s">
+        <v>165</v>
+      </c>
+      <c r="K8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B9" s="6" t="s">
         <v>42</v>
       </c>
@@ -1468,8 +1506,11 @@
       <c r="E9" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="H9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B10" s="6" t="s">
         <v>42</v>
       </c>
@@ -1480,8 +1521,11 @@
       <c r="E10" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="H10" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B11" s="6" t="s">
         <v>42</v>
       </c>
@@ -1490,8 +1534,11 @@
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="H11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B12" s="6" t="s">
         <v>42</v>
       </c>
@@ -1500,8 +1547,11 @@
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="2:5" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="H12" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" ht="52.2" x14ac:dyDescent="0.4">
       <c r="B13" s="6" t="s">
         <v>42</v>
       </c>
@@ -1513,7 +1563,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="2:5" ht="34.799999999999997" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:11" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="B14" s="6" t="s">
         <v>42</v>
       </c>
@@ -1525,7 +1575,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="2:5" ht="34.799999999999997" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:11" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="B15" s="6" t="s">
         <v>42</v>
       </c>
@@ -1537,7 +1587,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B16" s="6" t="s">
         <v>43</v>
       </c>
@@ -1661,7 +1711,7 @@
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B38" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="C38"/>
       <c r="D38"/>
@@ -1675,7 +1725,7 @@
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B40" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="C40"/>
       <c r="D40"/>
@@ -1689,25 +1739,25 @@
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B42" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="C42" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="D42" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="E42"/>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B43" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="C43" t="s">
         <v>21</v>
       </c>
       <c r="D43" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="E43"/>
     </row>
@@ -1717,27 +1767,27 @@
         <v>29</v>
       </c>
       <c r="D44" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="E44"/>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B45"/>
       <c r="C45" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="D45" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="E45"/>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B46"/>
       <c r="C46" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="D46" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="E46"/>
     </row>
@@ -1755,7 +1805,7 @@
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B49" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="C49"/>
       <c r="D49"/>
@@ -1769,10 +1819,10 @@
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B51" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="C51" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="D51"/>
       <c r="E51"/>
@@ -1780,14 +1830,136 @@
     <row r="52" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B52"/>
       <c r="C52" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="D52"/>
       <c r="E52"/>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C53" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B56" t="s">
+        <v>159</v>
+      </c>
+      <c r="C56"/>
+      <c r="D56"/>
+      <c r="E56"/>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B57" t="s">
+        <v>160</v>
+      </c>
+      <c r="C57"/>
+      <c r="D57"/>
+      <c r="E57"/>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B58" t="s">
+        <v>163</v>
+      </c>
+      <c r="C58"/>
+      <c r="D58"/>
+      <c r="E58"/>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B59" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="C59"/>
+      <c r="D59"/>
+      <c r="E59"/>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B60" t="s">
         <v>161</v>
+      </c>
+      <c r="C60"/>
+      <c r="D60" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B61" t="s">
+        <v>176</v>
+      </c>
+      <c r="C61"/>
+      <c r="D61"/>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B62" t="s">
+        <v>165</v>
+      </c>
+      <c r="C62"/>
+      <c r="D62" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B63" t="s">
+        <v>167</v>
+      </c>
+      <c r="C63"/>
+      <c r="D63"/>
+      <c r="E63"/>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B64" t="s">
+        <v>168</v>
+      </c>
+      <c r="C64"/>
+      <c r="D64"/>
+      <c r="E64"/>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B65" t="s">
+        <v>173</v>
+      </c>
+      <c r="C65"/>
+      <c r="D65" t="s">
+        <v>172</v>
+      </c>
+      <c r="E65"/>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B66" t="s">
+        <v>171</v>
+      </c>
+      <c r="C66"/>
+      <c r="D66"/>
+      <c r="E66"/>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B67" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B68" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B69" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B70" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B74" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -1813,7 +1985,7 @@
   <dimension ref="B1:F25"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1842,272 +2014,160 @@
         <v>5</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B5" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>55</v>
-      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B6" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>56</v>
-      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B7" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>57</v>
-      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B8" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>51</v>
-      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
-      <c r="F8" s="5" t="s">
-        <v>53</v>
-      </c>
+      <c r="F8" s="5"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B9" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>50</v>
-      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B10" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>60</v>
-      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B11" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>61</v>
-      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B12" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>62</v>
-      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B13" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>64</v>
-      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B14" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>65</v>
-      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B15" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>63</v>
-      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B16" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>68</v>
-      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B17" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>70</v>
-      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B18" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>58</v>
-      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B19" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>69</v>
-      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B20" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>71</v>
-      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="5"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B21" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>72</v>
-      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B22" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>74</v>
-      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
       <c r="D22" s="6"/>
-      <c r="E22" s="6" t="s">
-        <v>78</v>
-      </c>
+      <c r="E22" s="6"/>
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B23" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>75</v>
-      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
       <c r="D23" s="8"/>
-      <c r="E23" s="6" t="s">
-        <v>78</v>
-      </c>
+      <c r="E23" s="6"/>
       <c r="F23" s="8"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B24" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>76</v>
-      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
       <c r="D24" s="8"/>
-      <c r="E24" s="6" t="s">
-        <v>78</v>
-      </c>
+      <c r="E24" s="6"/>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B25" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>77</v>
-      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="6" t="s">
-        <v>78</v>
-      </c>
+      <c r="E25" s="6"/>
       <c r="F25" s="8"/>
     </row>
   </sheetData>
@@ -2141,16 +2201,16 @@
     <row r="1" spans="2:7" ht="12.6" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:7" ht="30" x14ac:dyDescent="0.4">
       <c r="B2" s="9" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="12.6" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="10" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
@@ -2159,10 +2219,10 @@
     </row>
     <row r="5" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="10" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
@@ -2171,10 +2231,10 @@
     </row>
     <row r="6" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="10" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
@@ -2183,13 +2243,13 @@
     </row>
     <row r="7" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="14" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>44</v>
@@ -2198,47 +2258,47 @@
         <v>42</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="6" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="21" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -2247,19 +2307,19 @@
         <v>Title</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="E10" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>120</v>
-      </c>
       <c r="G10" s="6" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -2268,79 +2328,79 @@
         <v>Title</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B12" s="6" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B13" s="6" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B14" s="22" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -2358,10 +2418,10 @@
       </c>
       <c r="E15" s="22"/>
       <c r="F15" s="6" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -2378,13 +2438,13 @@
         <v>Map (Day/Night)</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -2401,13 +2461,13 @@
         <v>Map (Day/Night)</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -2420,16 +2480,16 @@
         <v>Farm</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -2446,13 +2506,13 @@
         <v>Home</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -2465,16 +2525,16 @@
         <v>Farm</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -2491,13 +2551,13 @@
         <v>Animal House</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.4">
@@ -2506,19 +2566,19 @@
         <v>Play</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -2527,19 +2587,19 @@
         <v>Play</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -2552,16 +2612,16 @@
         <v>Pelican Town</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -2578,13 +2638,13 @@
         <v>Pierre's General Store</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -2597,16 +2657,16 @@
         <v>Pelican Town</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -2619,16 +2679,16 @@
         <v>Pelican Town</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -2637,19 +2697,19 @@
         <v>Play</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -2666,13 +2726,13 @@
         <v>Fish Shop</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.4">
@@ -2681,19 +2741,19 @@
         <v>Play</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -2702,19 +2762,19 @@
         <v>Play</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -2731,13 +2791,13 @@
         <v>First Floor</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -2750,16 +2810,16 @@
         <v>The Mines</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -2772,16 +2832,16 @@
         <v>The Mines</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -2794,16 +2854,16 @@
         <v>The Mines</v>
       </c>
       <c r="D35" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E35" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E35" s="6" t="s">
-        <v>117</v>
-      </c>
       <c r="F35" s="6" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -2816,16 +2876,16 @@
         <v>The Mines</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -2838,21 +2898,21 @@
         <v>The Mines</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B38" s="7" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="C38" s="8">
         <v>24</v>
@@ -2902,16 +2962,16 @@
     <row r="1" spans="2:6" ht="12.6" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:6" ht="30" x14ac:dyDescent="0.4">
       <c r="B2" s="9" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="12.6" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="2:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="10" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
@@ -2919,30 +2979,30 @@
     </row>
     <row r="5" spans="2:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="14" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="23" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C6" s="22" t="s">
         <v>46</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -2954,7 +3014,7 @@
       </c>
       <c r="C7" s="22"/>
       <c r="D7" s="6" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -2963,7 +3023,7 @@
       <c r="B8" s="24"/>
       <c r="C8" s="22"/>
       <c r="D8" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -2972,7 +3032,7 @@
       <c r="B9" s="24"/>
       <c r="C9" s="22"/>
       <c r="D9" s="6" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -3017,10 +3077,10 @@
         <v>Farm</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -3044,16 +3104,16 @@
         <v>Farm</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="2:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="25" t="str">
+      <c r="B17" s="27" t="str">
         <f t="shared" si="0"/>
         <v>Farm</v>
       </c>
@@ -3067,7 +3127,7 @@
     </row>
     <row r="18" spans="2:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B18" s="6" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>46</v>
@@ -3078,13 +3138,13 @@
     </row>
     <row r="19" spans="2:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B19" s="23" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>46</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
@@ -3095,10 +3155,10 @@
         <v>Pelican Town</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
@@ -3109,58 +3169,58 @@
         <v>#REF!</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
     </row>
     <row r="22" spans="2:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="25" t="e">
+      <c r="B22" s="27" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
     </row>
     <row r="23" spans="2:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B23" s="23" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>46</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
     </row>
     <row r="24" spans="2:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="25" t="str">
+      <c r="B24" s="27" t="str">
         <f>B23</f>
         <v>The Beach</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
     </row>
     <row r="25" spans="2:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B25" s="6" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>46</v>
@@ -3171,13 +3231,13 @@
     </row>
     <row r="26" spans="2:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B26" s="23" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
@@ -3192,7 +3252,7 @@
         <v>First Floor</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
@@ -3203,10 +3263,10 @@
         <v>The Mines</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
@@ -3215,7 +3275,7 @@
       <c r="B29" s="24"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
@@ -3226,10 +3286,10 @@
         <v>The Mines</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
@@ -3238,7 +3298,7 @@
       <c r="B31" s="24"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
@@ -3249,10 +3309,10 @@
         <v>The Mines</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
@@ -3261,7 +3321,7 @@
       <c r="B33" s="24"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
@@ -3269,45 +3329,45 @@
     <row r="34" spans="2:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B34" s="24"/>
       <c r="C34" s="6" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
     </row>
     <row r="35" spans="2:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="29"/>
+      <c r="B35" s="25"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
     </row>
     <row r="36" spans="2:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B36" s="29" t="str">
+      <c r="B36" s="25" t="str">
         <f>B32</f>
         <v>The Mines</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
     </row>
     <row r="37" spans="2:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B37" s="30" t="str">
+      <c r="B37" s="26" t="str">
         <f t="shared" si="0"/>
         <v>The Mines</v>
       </c>
       <c r="C37" s="6"/>
       <c r="D37" s="6" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
@@ -3315,15 +3375,15 @@
   </sheetData>
   <autoFilter ref="B5:E5" xr:uid="{4E32B991-2ACC-47FF-BF94-29DC9CD2AFBC}"/>
   <mergeCells count="9">
+    <mergeCell ref="C6:C13"/>
+    <mergeCell ref="B6:B17"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="B23:B24"/>
     <mergeCell ref="B26:B37"/>
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="B19:B22"/>
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C6:C13"/>
-    <mergeCell ref="B6:B17"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="B23:B24"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3335,7 +3395,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF74EBB9-74A1-4925-B94A-EB3F15421E86}">
   <dimension ref="B1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="B10" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -3351,16 +3411,16 @@
     <row r="1" spans="2:6" ht="12.6" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:6" ht="30" x14ac:dyDescent="0.4">
       <c r="B2" s="9" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="12.6" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="2:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="10" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
@@ -3368,42 +3428,42 @@
     </row>
     <row r="5" spans="2:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="14" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="23" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C6" s="22" t="s">
         <v>46</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="F6" s="6"/>
     </row>
     <row r="7" spans="2:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="24"/>
       <c r="C7" s="22"/>
-      <c r="D7" s="25"/>
+      <c r="D7" s="27"/>
       <c r="E7" s="6" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="F7" s="6"/>
     </row>
@@ -3414,19 +3474,19 @@
       </c>
       <c r="C8" s="22"/>
       <c r="D8" s="23" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="F8" s="6"/>
     </row>
     <row r="9" spans="2:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="24"/>
       <c r="C9" s="22"/>
-      <c r="D9" s="25"/>
+      <c r="D9" s="27"/>
       <c r="E9" s="6" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="F9" s="6"/>
     </row>
@@ -3434,19 +3494,19 @@
       <c r="B10" s="24"/>
       <c r="C10" s="22"/>
       <c r="D10" s="23" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="F10" s="6"/>
     </row>
     <row r="11" spans="2:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="24"/>
       <c r="C11" s="22"/>
-      <c r="D11" s="25"/>
+      <c r="D11" s="27"/>
       <c r="E11" s="6" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="F11" s="6"/>
     </row>
@@ -3454,19 +3514,19 @@
       <c r="B12" s="24"/>
       <c r="C12" s="22"/>
       <c r="D12" s="23" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="F12" s="6"/>
     </row>
     <row r="13" spans="2:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B13" s="24"/>
       <c r="C13" s="22"/>
-      <c r="D13" s="25"/>
+      <c r="D13" s="27"/>
       <c r="E13" s="6" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="F13" s="6"/>
     </row>
@@ -3476,13 +3536,13 @@
         <v>#REF!</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="F14" s="6"/>
     </row>
@@ -3492,13 +3552,13 @@
         <v>#REF!</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="F15" s="6"/>
     </row>
@@ -3507,52 +3567,52 @@
       <c r="C16" s="22"/>
       <c r="D16" s="24"/>
       <c r="E16" s="6" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="2:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="24"/>
       <c r="C17" s="22"/>
-      <c r="D17" s="25"/>
+      <c r="D17" s="27"/>
       <c r="E17" s="6" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="2:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B18" s="23" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="C18" s="23" t="s">
         <v>46</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="2:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
       <c r="E19" s="6" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="F19" s="6"/>
     </row>
     <row r="20" spans="2:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B20" s="23" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>46</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
@@ -3563,10 +3623,10 @@
         <v>Pelican Town</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
@@ -3577,58 +3637,58 @@
         <v>#REF!</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
     </row>
     <row r="23" spans="2:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="25" t="e">
+      <c r="B23" s="27" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
     </row>
     <row r="24" spans="2:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B24" s="23" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>46</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
     </row>
     <row r="25" spans="2:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="25" t="str">
+      <c r="B25" s="27" t="str">
         <f>B24</f>
         <v>The Beach</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
     </row>
     <row r="26" spans="2:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B26" s="6" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>46</v>
@@ -3639,13 +3699,13 @@
     </row>
     <row r="27" spans="2:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B27" s="23" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
@@ -3660,7 +3720,7 @@
         <v>First Floor</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
@@ -3671,10 +3731,10 @@
         <v>The Mines</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
@@ -3683,7 +3743,7 @@
       <c r="B30" s="24"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
@@ -3694,10 +3754,10 @@
         <v>The Mines</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
@@ -3706,7 +3766,7 @@
       <c r="B32" s="24"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
@@ -3717,10 +3777,10 @@
         <v>The Mines</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
@@ -3729,7 +3789,7 @@
       <c r="B34" s="24"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
@@ -3737,45 +3797,45 @@
     <row r="35" spans="2:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B35" s="24"/>
       <c r="C35" s="6" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
     </row>
     <row r="36" spans="2:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B36" s="29"/>
+      <c r="B36" s="25"/>
       <c r="C36" s="6"/>
       <c r="D36" s="6" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
     </row>
     <row r="37" spans="2:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B37" s="29" t="str">
+      <c r="B37" s="25" t="str">
         <f>B33</f>
         <v>The Mines</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
     </row>
     <row r="38" spans="2:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="30" t="str">
+      <c r="B38" s="26" t="str">
         <f t="shared" si="0"/>
         <v>The Mines</v>
       </c>
       <c r="C38" s="6"/>
       <c r="D38" s="6" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
@@ -3783,6 +3843,12 @@
   </sheetData>
   <autoFilter ref="B5:E5" xr:uid="{4E32B991-2ACC-47FF-BF94-29DC9CD2AFBC}"/>
   <mergeCells count="16">
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="B6:B17"/>
+    <mergeCell ref="C6:C13"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="D18:D19"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="B27:B38"/>
     <mergeCell ref="C27:C28"/>
@@ -3793,12 +3859,6 @@
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="B6:B17"/>
-    <mergeCell ref="C6:C13"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="D18:D19"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3825,7 +3885,7 @@
     <row r="1" spans="2:6" ht="12.6" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:6" ht="30" x14ac:dyDescent="0.4">
       <c r="B2" s="9" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -3833,63 +3893,63 @@
     <row r="3" spans="2:6" ht="12.6" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="28"/>
+        <v>144</v>
+      </c>
+      <c r="C4" s="28"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="30"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B5" s="7" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>42</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B6" s="6" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B7" s="6" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B8" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>

</xml_diff>